<commit_message>
Revert "Nose que onda"
This reverts commit 68eaa3905d2af64051f8ac9609891804376472c9.
</commit_message>
<xml_diff>
--- a/webroot/uploads/files/Test CRM - Cartera MACRO.xlsx
+++ b/webroot/uploads/files/Test CRM - Cartera MACRO.xlsx
@@ -85,6 +85,9 @@
     <t>Prestamo Personal</t>
   </si>
   <si>
+    <t>Pichi Sin Permisos</t>
+  </si>
+  <si>
     <t>Clelia Scapini</t>
   </si>
   <si>
@@ -140,9 +143,6 @@
   </si>
   <si>
     <t>SAN PEDRO</t>
-  </si>
-  <si>
-    <t>Pichi Sin Permisos</t>
   </si>
   <si>
     <t>Marta Maria Luisa Ruez</t>
@@ -422,7 +422,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -437,16 +437,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -456,17 +456,20 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -475,10 +478,10 @@
     <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -498,8 +501,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -698,17 +701,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -736,10 +739,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -987,12 +990,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1279,7 +1282,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1307,10 +1310,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1629,34 +1632,34 @@
       <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="P1" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="2">
+      <c r="Q1" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="R1" t="s" s="2">
+      <c r="R1" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="S1" t="s" s="2">
+      <c r="S1" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="T1" t="s" s="2">
+      <c r="T1" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="U1" t="s" s="2">
+      <c r="U1" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="V1" t="s" s="2">
+      <c r="V1" t="s" s="3">
         <v>15</v>
       </c>
     </row>
@@ -1664,7 +1667,7 @@
       <c r="A2" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>5383298</v>
       </c>
       <c r="C2" t="s" s="2">
@@ -1688,22 +1691,24 @@
       <c r="I2" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="4">
         <v>5400368758</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="5">
         <v>40821</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="4">
         <v>1947</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="6">
         <v>1672.47</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="6">
         <v>11868.08</v>
       </c>
-      <c r="O2" s="6"/>
+      <c r="O2" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P2" s="7">
         <v>2214241183</v>
       </c>
@@ -1722,42 +1727,44 @@
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4">
+        <v>4644243</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="J3" s="4">
+        <v>30255565</v>
+      </c>
+      <c r="K3" s="5">
+        <v>40674</v>
+      </c>
+      <c r="L3" s="4">
+        <v>2094</v>
+      </c>
+      <c r="M3" s="6">
+        <v>4373.17</v>
+      </c>
+      <c r="N3" s="6">
+        <v>19160.94</v>
+      </c>
+      <c r="O3" t="s" s="3">
         <v>24</v>
       </c>
-      <c r="B3" s="3">
-        <v>4644243</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3">
-        <v>30255565</v>
-      </c>
-      <c r="K3" s="4">
-        <v>40674</v>
-      </c>
-      <c r="L3" s="3">
-        <v>2094</v>
-      </c>
-      <c r="M3" s="5">
-        <v>4373.17</v>
-      </c>
-      <c r="N3" s="5">
-        <v>19160.94</v>
-      </c>
-      <c r="O3" s="2"/>
       <c r="P3" s="7">
         <v>0</v>
       </c>
@@ -1776,42 +1783,44 @@
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4">
         <v>13331793</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
       <c r="I4" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="4">
         <v>130107754</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="5">
         <v>40908</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="4">
         <v>1860</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="6">
         <v>773.54</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="6">
         <v>3559.45</v>
       </c>
-      <c r="O4" s="2"/>
+      <c r="O4" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P4" s="7">
         <v>3751420226</v>
       </c>
@@ -1830,42 +1839,44 @@
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B5" s="3">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4">
         <v>20489666</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
       <c r="I5" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="4">
         <v>20448153</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="5">
         <v>40827</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="4">
         <v>1941</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="6">
         <v>779.14</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="6">
         <v>3662.8</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P5" s="7">
         <v>0</v>
       </c>
@@ -1884,42 +1895,44 @@
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B6" s="3">
+        <v>35</v>
+      </c>
+      <c r="B6" s="4">
         <v>3562041</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
       <c r="I6" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="4">
         <v>310083944</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="5">
         <v>40554</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="4">
         <v>2214</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="6">
         <v>2420.75</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="6">
         <v>13625.07</v>
       </c>
-      <c r="O6" s="2"/>
+      <c r="O6" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P6" s="7">
         <v>3764470143</v>
       </c>
@@ -1938,42 +1951,44 @@
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B7" s="3">
+        <v>35</v>
+      </c>
+      <c r="B7" s="4">
         <v>3562041</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
       <c r="I7" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="4">
         <v>310088736</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="5">
         <v>40554</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="4">
         <v>2214</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="6">
         <v>4556.85</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="6">
         <v>25635.34</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P7" s="7">
         <v>3764470143</v>
       </c>
@@ -1992,42 +2007,44 @@
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B8" s="3">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4">
         <v>3562041</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
       <c r="I8" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="4">
         <v>310096965</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="5">
         <v>40554</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="4">
         <v>2214</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="6">
         <v>5835.62</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="6">
         <v>32842.52</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P8" s="7">
         <v>3764470143</v>
       </c>
@@ -2046,42 +2063,44 @@
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B9" s="3">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4">
         <v>3562041</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
       <c r="I9" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="4">
         <v>310097543</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="5">
         <v>40554</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="4">
         <v>2214</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="6">
         <v>1160.92</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="6">
         <v>6535.28</v>
       </c>
-      <c r="O9" s="2"/>
+      <c r="O9" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P9" s="7">
         <v>3764470143</v>
       </c>
@@ -2100,42 +2119,44 @@
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B10" s="3">
+        <v>35</v>
+      </c>
+      <c r="B10" s="4">
         <v>3562041</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
       <c r="I10" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="4">
         <v>310112012</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="5">
         <v>40554</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="4">
         <v>2212</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="6">
         <v>225.63</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="6">
         <v>1271.02</v>
       </c>
-      <c r="O10" s="2"/>
+      <c r="O10" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P10" s="7">
         <v>3764470143</v>
       </c>
@@ -2154,42 +2175,44 @@
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="B11" s="3">
+        <v>38</v>
+      </c>
+      <c r="B11" s="4">
         <v>4414245</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
       <c r="I11" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="4">
         <v>11049128</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="5">
         <v>40460</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="4">
         <v>2308</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="6">
         <v>346.44</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="6">
         <v>1661.25</v>
       </c>
-      <c r="O11" s="2"/>
+      <c r="O11" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P11" s="7">
         <v>3764467850</v>
       </c>
@@ -2208,42 +2231,44 @@
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="B12" s="3">
+        <v>38</v>
+      </c>
+      <c r="B12" s="4">
         <v>4414245</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
       <c r="I12" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="4">
         <v>140551639</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="5">
         <v>40460</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="4">
         <v>2275</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="6">
         <v>4953.93</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="6">
         <v>24037.68</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P12" s="7">
         <v>3764467850</v>
       </c>
@@ -2262,42 +2287,44 @@
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="B13" s="3">
+        <v>38</v>
+      </c>
+      <c r="B13" s="4">
         <v>4414245</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
       <c r="I13" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="4">
         <v>141013938</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="5">
         <v>40460</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="4">
         <v>2275</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="6">
         <v>914.86</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="6">
         <v>4428.75</v>
       </c>
-      <c r="O13" s="2"/>
+      <c r="O13" t="s" s="3">
+        <v>24</v>
+      </c>
       <c r="P13" s="7">
         <v>3764467850</v>
       </c>
@@ -2316,43 +2343,43 @@
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="B14" s="3">
+        <v>41</v>
+      </c>
+      <c r="B14" s="4">
         <v>5465760</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
       <c r="I14" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="4">
         <v>130063241</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="5">
         <v>40613</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="4">
         <v>2155</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="6">
         <v>2759.5</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="6">
         <v>13084.99</v>
       </c>
-      <c r="O14" t="s" s="2">
-        <v>43</v>
+      <c r="O14" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P14" s="7">
         <v>0</v>
@@ -2372,43 +2399,43 @@
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="B15" s="3">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4">
         <v>5465760</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
       <c r="I15" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="4">
         <v>130096078</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="5">
         <v>40613</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="4">
         <v>2122</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="6">
         <v>3354.21</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="6">
         <v>16129.16</v>
       </c>
-      <c r="O15" t="s" s="2">
-        <v>43</v>
+      <c r="O15" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P15" s="7">
         <v>0</v>
@@ -2428,43 +2455,43 @@
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="B16" s="3">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4">
         <v>5465760</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
       <c r="I16" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="4">
         <v>130109013</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="5">
         <v>40613</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="4">
         <v>2134</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="6">
         <v>1692.67</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="6">
         <v>8231.58</v>
       </c>
-      <c r="O16" t="s" s="2">
-        <v>43</v>
+      <c r="O16" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P16" s="7">
         <v>0</v>
@@ -2486,41 +2513,41 @@
       <c r="A17" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <v>5648419</v>
       </c>
       <c r="C17" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
       <c r="I17" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="4">
         <v>290181413</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="5">
         <v>40097</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17" s="4">
         <v>2671</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="6">
         <v>528.14</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="6">
         <v>4100.58</v>
       </c>
-      <c r="O17" t="s" s="2">
-        <v>43</v>
+      <c r="O17" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P17" s="7">
         <v>0</v>
@@ -2542,41 +2569,41 @@
       <c r="A18" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="4">
         <v>7588064</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>47</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
       <c r="I18" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="4">
         <v>90148245</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="5">
         <v>40425</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="4">
         <v>2336</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="6">
         <v>1668.96</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="6">
         <v>7529.45</v>
       </c>
-      <c r="O18" t="s" s="2">
-        <v>43</v>
+      <c r="O18" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P18" s="7">
         <v>3757421108</v>
@@ -2598,41 +2625,41 @@
       <c r="A19" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="4">
         <v>7588064</v>
       </c>
       <c r="C19" t="s" s="2">
         <v>47</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
       <c r="I19" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="4">
         <v>90156113</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="5">
         <v>40425</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="4">
         <v>2336</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="6">
         <v>1581.33</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="6">
         <v>7086.43</v>
       </c>
-      <c r="O19" t="s" s="2">
-        <v>43</v>
+      <c r="O19" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P19" s="7">
         <v>3757421108</v>
@@ -2654,41 +2681,41 @@
       <c r="A20" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="4">
         <v>7588064</v>
       </c>
       <c r="C20" t="s" s="2">
         <v>47</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
       <c r="I20" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="4">
         <v>90158317</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="5">
         <v>40425</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="4">
         <v>2336</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20" s="6">
         <v>1508.72</v>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="6">
         <v>6783.37</v>
       </c>
-      <c r="O20" t="s" s="2">
-        <v>43</v>
+      <c r="O20" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P20" s="7">
         <v>3757421108</v>
@@ -2710,41 +2737,41 @@
       <c r="A21" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <v>7588064</v>
       </c>
       <c r="C21" t="s" s="2">
         <v>47</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
       <c r="I21" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="4">
         <v>90168893</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="5">
         <v>40425</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="4">
         <v>2343</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21" s="6">
         <v>624.48</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="6">
         <v>2848.11</v>
       </c>
-      <c r="O21" t="s" s="2">
-        <v>43</v>
+      <c r="O21" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P21" s="7">
         <v>3757421108</v>
@@ -2766,41 +2793,41 @@
       <c r="A22" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>7588064</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>47</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
       <c r="I22" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="4">
         <v>90172272</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="5">
         <v>40425</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22" s="4">
         <v>2338</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="6">
         <v>785.52</v>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="6">
         <v>3621.97</v>
       </c>
-      <c r="O22" t="s" s="2">
-        <v>43</v>
+      <c r="O22" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P22" s="7">
         <v>3757421108</v>
@@ -2822,41 +2849,41 @@
       <c r="A23" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>7588064</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>47</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
       <c r="I23" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="4">
         <v>90172284</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="5">
         <v>40425</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23" s="4">
         <v>2338</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="6">
         <v>516.8200000000001</v>
       </c>
-      <c r="N23" s="5">
+      <c r="N23" s="6">
         <v>2382.62</v>
       </c>
-      <c r="O23" t="s" s="2">
-        <v>43</v>
+      <c r="O23" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P23" s="7">
         <v>3757421108</v>
@@ -2878,7 +2905,7 @@
       <c r="A24" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="4">
         <v>8561107</v>
       </c>
       <c r="C24" t="s" s="2">
@@ -2890,29 +2917,29 @@
       <c r="E24" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
       <c r="I24" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="4">
         <v>330105398</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="5">
         <v>40402</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24" s="4">
         <v>2366</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24" s="6">
         <v>560.55</v>
       </c>
-      <c r="N24" s="5">
+      <c r="N24" s="6">
         <v>3562.41</v>
       </c>
-      <c r="O24" t="s" s="2">
-        <v>43</v>
+      <c r="O24" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P24" s="7">
         <v>375615611069</v>
@@ -2934,41 +2961,41 @@
       <c r="A25" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="4">
         <v>10707642</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>54</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="I25" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="4">
         <v>90107928</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="5">
         <v>40543</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="4">
         <v>2183</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="6">
         <v>14219.91</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="6">
         <v>39801.25</v>
       </c>
-      <c r="O25" t="s" s="2">
-        <v>43</v>
+      <c r="O25" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P25" s="7">
         <v>0</v>
@@ -2990,41 +3017,41 @@
       <c r="A26" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>10707642</v>
       </c>
       <c r="C26" t="s" s="2">
         <v>54</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
       <c r="I26" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="4">
         <v>90181522</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="5">
         <v>40543</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26" s="4">
         <v>2225</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26" s="6">
         <v>736.3200000000001</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N26" s="6">
         <v>2104.83</v>
       </c>
-      <c r="O26" t="s" s="2">
-        <v>43</v>
+      <c r="O26" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P26" s="7">
         <v>0</v>
@@ -3046,41 +3073,41 @@
       <c r="A27" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="4">
         <v>10707642</v>
       </c>
       <c r="C27" t="s" s="2">
         <v>54</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E27" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
       <c r="I27" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="4">
         <v>90184794</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="5">
         <v>40543</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="4">
         <v>2150</v>
       </c>
-      <c r="M27" s="5">
+      <c r="M27" s="6">
         <v>155.73</v>
       </c>
-      <c r="N27" s="5">
+      <c r="N27" s="6">
         <v>444.22</v>
       </c>
-      <c r="O27" t="s" s="2">
-        <v>43</v>
+      <c r="O27" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P27" s="7">
         <v>0</v>
@@ -3102,41 +3129,41 @@
       <c r="A28" t="s" s="2">
         <v>55</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="4">
         <v>11313444</v>
       </c>
       <c r="C28" t="s" s="2">
         <v>56</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
       <c r="I28" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="4">
         <v>140795479</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="5">
         <v>40036</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28" s="4">
         <v>2732</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28" s="6">
         <v>23300.35</v>
       </c>
-      <c r="N28" s="5">
+      <c r="N28" s="6">
         <v>70840.039999999994</v>
       </c>
-      <c r="O28" t="s" s="2">
-        <v>43</v>
+      <c r="O28" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P28" s="7">
         <v>0</v>
@@ -3158,41 +3185,41 @@
       <c r="A29" t="s" s="2">
         <v>57</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="4">
         <v>12416484</v>
       </c>
       <c r="C29" t="s" s="2">
         <v>58</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E29" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
       <c r="I29" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="4">
         <v>110039169</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="5">
         <v>40462</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29" s="4">
         <v>2306</v>
       </c>
-      <c r="M29" s="5">
+      <c r="M29" s="6">
         <v>9411.360000000001</v>
       </c>
-      <c r="N29" s="5">
+      <c r="N29" s="6">
         <v>29698.37</v>
       </c>
-      <c r="O29" t="s" s="2">
-        <v>43</v>
+      <c r="O29" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P29" s="7">
         <v>3758422638</v>
@@ -3214,41 +3241,41 @@
       <c r="A30" t="s" s="2">
         <v>57</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="4">
         <v>12416484</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>58</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E30" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
       <c r="I30" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="4">
         <v>110059494</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30" s="5">
         <v>40462</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30" s="4">
         <v>2275</v>
       </c>
-      <c r="M30" s="5">
+      <c r="M30" s="6">
         <v>319.51</v>
       </c>
-      <c r="N30" s="5">
+      <c r="N30" s="6">
         <v>1027.33</v>
       </c>
-      <c r="O30" t="s" s="2">
-        <v>43</v>
+      <c r="O30" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P30" s="7">
         <v>3758422638</v>
@@ -3270,41 +3297,41 @@
       <c r="A31" t="s" s="2">
         <v>57</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>12416484</v>
       </c>
       <c r="C31" t="s" s="2">
         <v>58</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
       <c r="I31" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="4">
         <v>110063017</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K31" s="5">
         <v>40462</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="4">
         <v>2306</v>
       </c>
-      <c r="M31" s="5">
+      <c r="M31" s="6">
         <v>4909.97</v>
       </c>
-      <c r="N31" s="5">
+      <c r="N31" s="6">
         <v>15375.71</v>
       </c>
-      <c r="O31" t="s" s="2">
-        <v>43</v>
+      <c r="O31" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P31" s="7">
         <v>3758422638</v>
@@ -3326,41 +3353,41 @@
       <c r="A32" t="s" s="2">
         <v>60</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="4">
         <v>12834126</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>61</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E32" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
       <c r="I32" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="4">
         <v>310135026</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K32" s="5">
         <v>40857</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32" s="4">
         <v>1911</v>
       </c>
-      <c r="M32" s="5">
+      <c r="M32" s="6">
         <v>48375.88</v>
       </c>
-      <c r="N32" s="5">
+      <c r="N32" s="6">
         <v>23368.41</v>
       </c>
-      <c r="O32" t="s" s="2">
-        <v>43</v>
+      <c r="O32" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P32" s="7">
         <v>3764470406</v>
@@ -3382,7 +3409,7 @@
       <c r="A33" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="4">
         <v>14968832</v>
       </c>
       <c r="C33" t="s" s="2">
@@ -3394,29 +3421,29 @@
       <c r="E33" t="s" s="2">
         <v>65</v>
       </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
       <c r="I33" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="4">
         <v>3010254655</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K33" s="5">
         <v>40402</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33" s="4">
         <v>2366</v>
       </c>
-      <c r="M33" s="5">
+      <c r="M33" s="6">
         <v>3609.47</v>
       </c>
-      <c r="N33" s="5">
+      <c r="N33" s="6">
         <v>22931.22</v>
       </c>
-      <c r="O33" t="s" s="2">
-        <v>43</v>
+      <c r="O33" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P33" s="7">
         <v>354115612478</v>
@@ -3438,41 +3465,41 @@
       <c r="A34" t="s" s="2">
         <v>66</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="4">
         <v>16442823</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>67</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
       <c r="I34" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="4">
         <v>140827260</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="5">
         <v>40220</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34" s="4">
         <v>2548</v>
       </c>
-      <c r="M34" s="5">
+      <c r="M34" s="6">
         <v>16656.02</v>
       </c>
-      <c r="N34" s="5">
+      <c r="N34" s="6">
         <v>86686.820000000007</v>
       </c>
-      <c r="O34" t="s" s="2">
-        <v>43</v>
+      <c r="O34" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P34" s="7">
         <v>0</v>
@@ -3494,41 +3521,41 @@
       <c r="A35" t="s" s="2">
         <v>68</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="4">
         <v>18283368</v>
       </c>
       <c r="C35" t="s" s="2">
         <v>69</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E35" t="s" s="2">
         <v>70</v>
       </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
       <c r="I35" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="4">
         <v>11065861</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K35" s="5">
         <v>40513</v>
       </c>
-      <c r="L35" s="3">
+      <c r="L35" s="4">
         <v>2255</v>
       </c>
-      <c r="M35" s="5">
+      <c r="M35" s="6">
         <v>620.09</v>
       </c>
-      <c r="N35" s="5">
+      <c r="N35" s="6">
         <v>2676.63</v>
       </c>
-      <c r="O35" t="s" s="2">
-        <v>43</v>
+      <c r="O35" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P35" s="7">
         <v>376154519564</v>
@@ -3550,41 +3577,41 @@
       <c r="A36" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="4">
         <v>20987099</v>
       </c>
       <c r="C36" t="s" s="2">
         <v>72</v>
       </c>
       <c r="D36" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E36" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
       <c r="I36" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="4">
         <v>10812204</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36" s="5">
         <v>40766</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36" s="4">
         <v>1910</v>
       </c>
-      <c r="M36" s="5">
+      <c r="M36" s="6">
         <v>4834.32</v>
       </c>
-      <c r="N36" s="5">
+      <c r="N36" s="6">
         <v>21279.09</v>
       </c>
-      <c r="O36" t="s" s="2">
-        <v>43</v>
+      <c r="O36" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P36" s="7">
         <v>0</v>
@@ -3606,41 +3633,41 @@
       <c r="A37" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="4">
         <v>20987099</v>
       </c>
       <c r="C37" t="s" s="2">
         <v>72</v>
       </c>
       <c r="D37" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E37" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
       <c r="I37" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="4">
         <v>10852137</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37" s="5">
         <v>40766</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37" s="4">
         <v>1971</v>
       </c>
-      <c r="M37" s="5">
+      <c r="M37" s="6">
         <v>7165.76</v>
       </c>
-      <c r="N37" s="5">
+      <c r="N37" s="6">
         <v>31493.43</v>
       </c>
-      <c r="O37" t="s" s="2">
-        <v>43</v>
+      <c r="O37" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P37" s="7">
         <v>0</v>
@@ -3662,41 +3689,41 @@
       <c r="A38" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="4">
         <v>20987099</v>
       </c>
       <c r="C38" t="s" s="2">
         <v>72</v>
       </c>
       <c r="D38" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E38" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
       <c r="I38" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="4">
         <v>10898234</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="5">
         <v>40766</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="4">
         <v>2002</v>
       </c>
-      <c r="M38" s="5">
+      <c r="M38" s="6">
         <v>7009.1</v>
       </c>
-      <c r="N38" s="5">
+      <c r="N38" s="6">
         <v>30543.9</v>
       </c>
-      <c r="O38" t="s" s="2">
-        <v>43</v>
+      <c r="O38" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P38" s="7">
         <v>0</v>
@@ -3718,41 +3745,41 @@
       <c r="A39" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="4">
         <v>20987099</v>
       </c>
       <c r="C39" t="s" s="2">
         <v>72</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
       <c r="I39" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="4">
         <v>11156531</v>
       </c>
-      <c r="K39" s="4">
+      <c r="K39" s="5">
         <v>40766</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L39" s="4">
         <v>1918</v>
       </c>
-      <c r="M39" s="5">
+      <c r="M39" s="6">
         <v>189.8</v>
       </c>
-      <c r="N39" s="5">
+      <c r="N39" s="6">
         <v>828.3099999999999</v>
       </c>
-      <c r="O39" t="s" s="2">
-        <v>43</v>
+      <c r="O39" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P39" s="7">
         <v>0</v>
@@ -3774,7 +3801,7 @@
       <c r="A40" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="4">
         <v>25284155</v>
       </c>
       <c r="C40" t="s" s="2">
@@ -3786,29 +3813,29 @@
       <c r="E40" t="s" s="2">
         <v>75</v>
       </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
       <c r="I40" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="4">
         <v>5400231242</v>
       </c>
-      <c r="K40" s="4">
+      <c r="K40" s="5">
         <v>40426</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40" s="4">
         <v>2342</v>
       </c>
-      <c r="M40" s="5">
+      <c r="M40" s="6">
         <v>2434.29</v>
       </c>
-      <c r="N40" s="5">
+      <c r="N40" s="6">
         <v>15157.76</v>
       </c>
-      <c r="O40" t="s" s="2">
-        <v>43</v>
+      <c r="O40" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P40" s="7">
         <v>1147392034</v>
@@ -3830,7 +3857,7 @@
       <c r="A41" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="4">
         <v>25706370</v>
       </c>
       <c r="C41" t="s" s="2">
@@ -3842,29 +3869,29 @@
       <c r="E41" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
       <c r="I41" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="4">
         <v>5130031303</v>
       </c>
-      <c r="K41" s="4">
+      <c r="K41" s="5">
         <v>40248</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L41" s="4">
         <v>2520</v>
       </c>
-      <c r="M41" s="5">
+      <c r="M41" s="6">
         <v>757.88</v>
       </c>
-      <c r="N41" s="5">
+      <c r="N41" s="6">
         <v>5257.39</v>
       </c>
-      <c r="O41" t="s" s="2">
-        <v>43</v>
+      <c r="O41" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P41" s="7">
         <v>1142629411</v>
@@ -3886,41 +3913,41 @@
       <c r="A42" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="4">
         <v>29830054</v>
       </c>
       <c r="C42" t="s" s="2">
         <v>80</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E42" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
       <c r="I42" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="4">
         <v>10894654</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="5">
         <v>40128</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L42" s="4">
         <v>2640</v>
       </c>
-      <c r="M42" s="5">
+      <c r="M42" s="6">
         <v>1543.59</v>
       </c>
-      <c r="N42" s="5">
+      <c r="N42" s="6">
         <v>15503.51</v>
       </c>
-      <c r="O42" t="s" s="2">
-        <v>43</v>
+      <c r="O42" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P42" s="7">
         <v>376154739663</v>
@@ -3942,41 +3969,41 @@
       <c r="A43" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="4">
         <v>17786628</v>
       </c>
       <c r="C43" t="s" s="2">
         <v>82</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E43" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
       <c r="I43" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="4">
         <v>160032159</v>
       </c>
-      <c r="K43" s="4">
+      <c r="K43" s="5">
         <v>40858</v>
       </c>
-      <c r="L43" s="3">
+      <c r="L43" s="4">
         <v>1910</v>
       </c>
-      <c r="M43" s="5">
+      <c r="M43" s="6">
         <v>786.0700000000001</v>
       </c>
-      <c r="N43" s="5">
+      <c r="N43" s="6">
         <v>3485.2</v>
       </c>
-      <c r="O43" t="s" s="2">
-        <v>43</v>
+      <c r="O43" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P43" s="7">
         <v>3758470214</v>
@@ -3998,41 +4025,41 @@
       <c r="A44" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="4">
         <v>18592459</v>
       </c>
       <c r="C44" t="s" s="2">
         <v>85</v>
       </c>
       <c r="D44" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E44" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
       <c r="I44" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="4">
         <v>141161620</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K44" s="5">
         <v>40857</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L44" s="4">
         <v>1911</v>
       </c>
-      <c r="M44" s="5">
+      <c r="M44" s="6">
         <v>4822.23</v>
       </c>
-      <c r="N44" s="5">
+      <c r="N44" s="6">
         <v>30073.2</v>
       </c>
-      <c r="O44" t="s" s="2">
-        <v>43</v>
+      <c r="O44" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P44" s="7">
         <v>376154355490</v>
@@ -4054,41 +4081,41 @@
       <c r="A45" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="4">
         <v>18154786</v>
       </c>
       <c r="C45" t="s" s="2">
         <v>87</v>
       </c>
       <c r="D45" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E45" t="s" s="2">
         <v>70</v>
       </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
       <c r="I45" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="4">
         <v>140398609</v>
       </c>
-      <c r="K45" s="4">
+      <c r="K45" s="5">
         <v>40370</v>
       </c>
-      <c r="L45" s="3">
+      <c r="L45" s="4">
         <v>2398</v>
       </c>
-      <c r="M45" s="5">
+      <c r="M45" s="6">
         <v>4356.84</v>
       </c>
-      <c r="N45" s="5">
+      <c r="N45" s="6">
         <v>23714.1</v>
       </c>
-      <c r="O45" t="s" s="2">
-        <v>43</v>
+      <c r="O45" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P45" s="7">
         <v>376154238251</v>
@@ -4110,41 +4137,41 @@
       <c r="A46" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="4">
         <v>18154786</v>
       </c>
       <c r="C46" t="s" s="2">
         <v>87</v>
       </c>
       <c r="D46" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E46" t="s" s="2">
         <v>70</v>
       </c>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
       <c r="I46" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="4">
         <v>140965177</v>
       </c>
-      <c r="K46" s="4">
+      <c r="K46" s="5">
         <v>40370</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L46" s="4">
         <v>2394</v>
       </c>
-      <c r="M46" s="5">
+      <c r="M46" s="6">
         <v>1656.89</v>
       </c>
-      <c r="N46" s="5">
+      <c r="N46" s="6">
         <v>9021.42</v>
       </c>
-      <c r="O46" t="s" s="2">
-        <v>43</v>
+      <c r="O46" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P46" s="7">
         <v>376154238251</v>
@@ -4166,41 +4193,41 @@
       <c r="A47" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="4">
         <v>7540447</v>
       </c>
       <c r="C47" t="s" s="2">
         <v>89</v>
       </c>
       <c r="D47" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E47" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
       <c r="I47" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="4">
         <v>310115222</v>
       </c>
-      <c r="K47" s="4">
+      <c r="K47" s="5">
         <v>40940</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47" s="4">
         <v>1818</v>
       </c>
-      <c r="M47" s="5">
+      <c r="M47" s="6">
         <v>18494.07</v>
       </c>
-      <c r="N47" s="5">
+      <c r="N47" s="6">
         <v>53824.98</v>
       </c>
-      <c r="O47" t="s" s="2">
-        <v>43</v>
+      <c r="O47" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P47" s="7">
         <v>3764497194</v>
@@ -4222,41 +4249,41 @@
       <c r="A48" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="4">
         <v>7540447</v>
       </c>
       <c r="C48" t="s" s="2">
         <v>89</v>
       </c>
       <c r="D48" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E48" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
       <c r="I48" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="4">
         <v>310140564</v>
       </c>
-      <c r="K48" s="4">
+      <c r="K48" s="5">
         <v>40940</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48" s="4">
         <v>1818</v>
       </c>
-      <c r="M48" s="5">
+      <c r="M48" s="6">
         <v>3978.27</v>
       </c>
-      <c r="N48" s="5">
+      <c r="N48" s="6">
         <v>11877.15</v>
       </c>
-      <c r="O48" t="s" s="2">
-        <v>43</v>
+      <c r="O48" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P48" s="7">
         <v>3764497194</v>
@@ -4278,41 +4305,41 @@
       <c r="A49" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="4">
         <v>7540447</v>
       </c>
       <c r="C49" t="s" s="2">
         <v>89</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E49" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
       <c r="I49" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="4">
         <v>310142108</v>
       </c>
-      <c r="K49" s="4">
+      <c r="K49" s="5">
         <v>40940</v>
       </c>
-      <c r="L49" s="3">
+      <c r="L49" s="4">
         <v>1828</v>
       </c>
-      <c r="M49" s="5">
+      <c r="M49" s="6">
         <v>209.02</v>
       </c>
-      <c r="N49" s="5">
+      <c r="N49" s="6">
         <v>623.97</v>
       </c>
-      <c r="O49" t="s" s="2">
-        <v>43</v>
+      <c r="O49" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P49" s="7">
         <v>3764497194</v>
@@ -4334,41 +4361,41 @@
       <c r="A50" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="4">
         <v>24239725</v>
       </c>
       <c r="C50" t="s" s="2">
         <v>92</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E50" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
       <c r="I50" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="4">
         <v>20548525</v>
       </c>
-      <c r="K50" s="4">
+      <c r="K50" s="5">
         <v>40829</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50" s="4">
         <v>1939</v>
       </c>
-      <c r="M50" s="5">
+      <c r="M50" s="6">
         <v>1600.45</v>
       </c>
-      <c r="N50" s="5">
+      <c r="N50" s="6">
         <v>10366.14</v>
       </c>
-      <c r="O50" t="s" s="2">
-        <v>43</v>
+      <c r="O50" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P50" s="7">
         <v>376154641128</v>
@@ -4390,7 +4417,7 @@
       <c r="A51" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="4">
         <v>20806002</v>
       </c>
       <c r="C51" t="s" s="2">
@@ -4402,29 +4429,29 @@
       <c r="E51" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
       <c r="I51" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="4">
         <v>7830026614</v>
       </c>
-      <c r="K51" s="4">
+      <c r="K51" s="5">
         <v>40870</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51" s="4">
         <v>1880</v>
       </c>
-      <c r="M51" s="5">
+      <c r="M51" s="6">
         <v>8346.02</v>
       </c>
-      <c r="N51" s="5">
+      <c r="N51" s="6">
         <v>36941.94</v>
       </c>
-      <c r="O51" t="s" s="2">
-        <v>43</v>
+      <c r="O51" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P51" s="7">
         <v>347615642664</v>
@@ -4446,7 +4473,7 @@
       <c r="A52" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="4">
         <v>20806002</v>
       </c>
       <c r="C52" t="s" s="2">
@@ -4458,29 +4485,29 @@
       <c r="E52" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
       <c r="I52" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="4">
         <v>7830034922</v>
       </c>
-      <c r="K52" s="4">
+      <c r="K52" s="5">
         <v>40870</v>
       </c>
-      <c r="L52" s="3">
+      <c r="L52" s="4">
         <v>1876</v>
       </c>
-      <c r="M52" s="5">
+      <c r="M52" s="6">
         <v>674.11</v>
       </c>
-      <c r="N52" s="5">
+      <c r="N52" s="6">
         <v>2983.35</v>
       </c>
-      <c r="O52" t="s" s="2">
-        <v>43</v>
+      <c r="O52" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P52" s="7">
         <v>347615642664</v>
@@ -4502,7 +4529,7 @@
       <c r="A53" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="4">
         <v>20806002</v>
       </c>
       <c r="C53" t="s" s="2">
@@ -4514,29 +4541,29 @@
       <c r="E53" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
       <c r="I53" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="4">
         <v>7830036396</v>
       </c>
-      <c r="K53" s="4">
+      <c r="K53" s="5">
         <v>40870</v>
       </c>
-      <c r="L53" s="3">
+      <c r="L53" s="4">
         <v>1898</v>
       </c>
-      <c r="M53" s="5">
+      <c r="M53" s="6">
         <v>2063.47</v>
       </c>
-      <c r="N53" s="5">
+      <c r="N53" s="6">
         <v>9199.48</v>
       </c>
-      <c r="O53" t="s" s="2">
-        <v>43</v>
+      <c r="O53" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P53" s="7">
         <v>347615642664</v>
@@ -4558,7 +4585,7 @@
       <c r="A54" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="4">
         <v>11136443</v>
       </c>
       <c r="C54" t="s" s="2">
@@ -4570,29 +4597,29 @@
       <c r="E54" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
       <c r="I54" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54" s="4">
         <v>1002839313</v>
       </c>
-      <c r="K54" s="4">
+      <c r="K54" s="5">
         <v>40740</v>
       </c>
-      <c r="L54" s="3">
+      <c r="L54" s="4">
         <v>2028</v>
       </c>
-      <c r="M54" s="5">
+      <c r="M54" s="6">
         <v>14362.12</v>
       </c>
-      <c r="N54" s="5">
+      <c r="N54" s="6">
         <v>74926.14</v>
       </c>
-      <c r="O54" t="s" s="2">
-        <v>43</v>
+      <c r="O54" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P54" s="7">
         <v>3874316518</v>
@@ -4614,7 +4641,7 @@
       <c r="A55" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="4">
         <v>11136443</v>
       </c>
       <c r="C55" t="s" s="2">
@@ -4626,29 +4653,29 @@
       <c r="E55" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
       <c r="I55" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J55" s="4">
         <v>1002997634</v>
       </c>
-      <c r="K55" s="4">
+      <c r="K55" s="5">
         <v>40740</v>
       </c>
-      <c r="L55" s="3">
+      <c r="L55" s="4">
         <v>2028</v>
       </c>
-      <c r="M55" s="5">
+      <c r="M55" s="6">
         <v>6449.92</v>
       </c>
-      <c r="N55" s="5">
+      <c r="N55" s="6">
         <v>33645.8</v>
       </c>
-      <c r="O55" t="s" s="2">
-        <v>43</v>
+      <c r="O55" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P55" s="7">
         <v>3874316518</v>
@@ -4670,7 +4697,7 @@
       <c r="A56" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="4">
         <v>11136443</v>
       </c>
       <c r="C56" t="s" s="2">
@@ -4682,29 +4709,29 @@
       <c r="E56" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
       <c r="I56" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="4">
         <v>1003454421</v>
       </c>
-      <c r="K56" s="4">
+      <c r="K56" s="5">
         <v>40740</v>
       </c>
-      <c r="L56" s="3">
+      <c r="L56" s="4">
         <v>2017</v>
       </c>
-      <c r="M56" s="5">
+      <c r="M56" s="6">
         <v>2457.03</v>
       </c>
-      <c r="N56" s="5">
+      <c r="N56" s="6">
         <v>12815.26</v>
       </c>
-      <c r="O56" t="s" s="2">
-        <v>43</v>
+      <c r="O56" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P56" s="7">
         <v>3874316518</v>
@@ -4726,7 +4753,7 @@
       <c r="A57" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="4">
         <v>11834714</v>
       </c>
       <c r="C57" t="s" s="2">
@@ -4738,29 +4765,29 @@
       <c r="E57" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
       <c r="I57" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J57" s="4">
         <v>1001675174</v>
       </c>
-      <c r="K57" s="4">
+      <c r="K57" s="5">
         <v>40309</v>
       </c>
-      <c r="L57" s="3">
+      <c r="L57" s="4">
         <v>2459</v>
       </c>
-      <c r="M57" s="5">
+      <c r="M57" s="6">
         <v>7756.46</v>
       </c>
-      <c r="N57" s="5">
+      <c r="N57" s="6">
         <v>39787.06</v>
       </c>
-      <c r="O57" t="s" s="2">
-        <v>43</v>
+      <c r="O57" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P57" s="7">
         <v>387154743688</v>
@@ -4782,7 +4809,7 @@
       <c r="A58" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="4">
         <v>11834714</v>
       </c>
       <c r="C58" t="s" s="2">
@@ -4794,29 +4821,29 @@
       <c r="E58" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
       <c r="I58" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J58" s="4">
         <v>1001822870</v>
       </c>
-      <c r="K58" s="4">
+      <c r="K58" s="5">
         <v>40309</v>
       </c>
-      <c r="L58" s="3">
+      <c r="L58" s="4">
         <v>2459</v>
       </c>
-      <c r="M58" s="5">
+      <c r="M58" s="6">
         <v>984.63</v>
       </c>
-      <c r="N58" s="5">
+      <c r="N58" s="6">
         <v>5050.48</v>
       </c>
-      <c r="O58" t="s" s="2">
-        <v>43</v>
+      <c r="O58" t="s" s="3">
+        <v>24</v>
       </c>
       <c r="P58" s="7">
         <v>387154743688</v>
@@ -4838,7 +4865,7 @@
       <c r="A59" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="4">
         <v>11834714</v>
       </c>
       <c r="C59" t="s" s="2">
@@ -4850,28 +4877,28 @@
       <c r="E59" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
       <c r="I59" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J59" s="3">
+      <c r="J59" s="4">
         <v>1002504190</v>
       </c>
-      <c r="K59" s="4">
+      <c r="K59" s="5">
         <v>40309</v>
       </c>
-      <c r="L59" s="3">
+      <c r="L59" s="4">
         <v>2459</v>
       </c>
-      <c r="M59" s="5">
+      <c r="M59" s="6">
         <v>363.15</v>
       </c>
-      <c r="N59" s="5">
+      <c r="N59" s="6">
         <v>1852.58</v>
       </c>
-      <c r="O59" t="s" s="2">
+      <c r="O59" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P59" s="7">
@@ -4894,7 +4921,7 @@
       <c r="A60" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="4">
         <v>17196845</v>
       </c>
       <c r="C60" t="s" s="2">
@@ -4906,28 +4933,28 @@
       <c r="E60" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
       <c r="I60" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J60" s="3">
+      <c r="J60" s="4">
         <v>1001831053</v>
       </c>
-      <c r="K60" s="4">
+      <c r="K60" s="5">
         <v>40520</v>
       </c>
-      <c r="L60" s="3">
+      <c r="L60" s="4">
         <v>2245</v>
       </c>
-      <c r="M60" s="5">
+      <c r="M60" s="6">
         <v>1338.45</v>
       </c>
-      <c r="N60" s="5">
+      <c r="N60" s="6">
         <v>5545.85</v>
       </c>
-      <c r="O60" t="s" s="2">
+      <c r="O60" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P60" s="7">
@@ -4950,7 +4977,7 @@
       <c r="A61" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="4">
         <v>17196845</v>
       </c>
       <c r="C61" t="s" s="2">
@@ -4962,28 +4989,28 @@
       <c r="E61" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
       <c r="I61" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J61" s="3">
+      <c r="J61" s="4">
         <v>1003192853</v>
       </c>
-      <c r="K61" s="4">
+      <c r="K61" s="5">
         <v>40520</v>
       </c>
-      <c r="L61" s="3">
+      <c r="L61" s="4">
         <v>2248</v>
       </c>
-      <c r="M61" s="5">
+      <c r="M61" s="6">
         <v>1226.12</v>
       </c>
-      <c r="N61" s="5">
+      <c r="N61" s="6">
         <v>5175.1</v>
       </c>
-      <c r="O61" t="s" s="2">
+      <c r="O61" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P61" s="7">
@@ -5006,7 +5033,7 @@
       <c r="A62" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="4">
         <v>17196845</v>
       </c>
       <c r="C62" t="s" s="2">
@@ -5018,28 +5045,28 @@
       <c r="E62" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
       <c r="I62" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J62" s="4">
         <v>1490010275</v>
       </c>
-      <c r="K62" s="4">
+      <c r="K62" s="5">
         <v>40520</v>
       </c>
-      <c r="L62" s="3">
+      <c r="L62" s="4">
         <v>2245</v>
       </c>
-      <c r="M62" s="5">
+      <c r="M62" s="6">
         <v>5806.08</v>
       </c>
-      <c r="N62" s="5">
+      <c r="N62" s="6">
         <v>24132.29</v>
       </c>
-      <c r="O62" t="s" s="2">
+      <c r="O62" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P62" s="7">
@@ -5062,7 +5089,7 @@
       <c r="A63" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="4">
         <v>17196845</v>
       </c>
       <c r="C63" t="s" s="2">
@@ -5074,28 +5101,28 @@
       <c r="E63" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
       <c r="I63" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J63" s="3">
+      <c r="J63" s="4">
         <v>1490027759</v>
       </c>
-      <c r="K63" s="4">
+      <c r="K63" s="5">
         <v>40520</v>
       </c>
-      <c r="L63" s="3">
+      <c r="L63" s="4">
         <v>2245</v>
       </c>
-      <c r="M63" s="5">
+      <c r="M63" s="6">
         <v>8809.73</v>
       </c>
-      <c r="N63" s="5">
+      <c r="N63" s="6">
         <v>36493.58</v>
       </c>
-      <c r="O63" t="s" s="2">
+      <c r="O63" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P63" s="7">
@@ -5118,7 +5145,7 @@
       <c r="A64" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="4">
         <v>17196845</v>
       </c>
       <c r="C64" t="s" s="2">
@@ -5130,28 +5157,28 @@
       <c r="E64" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
       <c r="I64" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J64" s="3">
+      <c r="J64" s="4">
         <v>1490044666</v>
       </c>
-      <c r="K64" s="4">
+      <c r="K64" s="5">
         <v>40520</v>
       </c>
-      <c r="L64" s="3">
+      <c r="L64" s="4">
         <v>2233</v>
       </c>
-      <c r="M64" s="5">
+      <c r="M64" s="6">
         <v>1790.15</v>
       </c>
-      <c r="N64" s="5">
+      <c r="N64" s="6">
         <v>7579.84</v>
       </c>
-      <c r="O64" t="s" s="2">
+      <c r="O64" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P64" s="7">
@@ -5174,7 +5201,7 @@
       <c r="A65" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="4">
         <v>18229220</v>
       </c>
       <c r="C65" t="s" s="2">
@@ -5186,28 +5213,28 @@
       <c r="E65" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
       <c r="I65" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J65" s="3">
+      <c r="J65" s="4">
         <v>1003227402</v>
       </c>
-      <c r="K65" s="4">
+      <c r="K65" s="5">
         <v>40858</v>
       </c>
-      <c r="L65" s="3">
+      <c r="L65" s="4">
         <v>1910</v>
       </c>
-      <c r="M65" s="5">
+      <c r="M65" s="6">
         <v>12812.18</v>
       </c>
-      <c r="N65" s="5">
+      <c r="N65" s="6">
         <v>50014.82</v>
       </c>
-      <c r="O65" t="s" s="2">
+      <c r="O65" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P65" s="7">
@@ -5230,7 +5257,7 @@
       <c r="A66" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="4">
         <v>6344067</v>
       </c>
       <c r="C66" t="s" s="2">
@@ -5242,28 +5269,28 @@
       <c r="E66" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
       <c r="I66" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J66" s="3">
+      <c r="J66" s="4">
         <v>1003164167</v>
       </c>
-      <c r="K66" s="4">
+      <c r="K66" s="5">
         <v>40494</v>
       </c>
-      <c r="L66" s="3">
+      <c r="L66" s="4">
         <v>2274</v>
       </c>
-      <c r="M66" s="5">
+      <c r="M66" s="6">
         <v>696.61</v>
       </c>
-      <c r="N66" s="5">
+      <c r="N66" s="6">
         <v>8880.74</v>
       </c>
-      <c r="O66" t="s" s="2">
+      <c r="O66" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P66" s="7">
@@ -5286,7 +5313,7 @@
       <c r="A67" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="4">
         <v>3689386</v>
       </c>
       <c r="C67" t="s" s="2">
@@ -5298,28 +5325,28 @@
       <c r="E67" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
       <c r="I67" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J67" s="3">
+      <c r="J67" s="4">
         <v>1003252287</v>
       </c>
-      <c r="K67" s="4">
+      <c r="K67" s="5">
         <v>40577</v>
       </c>
-      <c r="L67" s="3">
+      <c r="L67" s="4">
         <v>2191</v>
       </c>
-      <c r="M67" s="5">
+      <c r="M67" s="6">
         <v>808.5599999999999</v>
       </c>
-      <c r="N67" s="5">
+      <c r="N67" s="6">
         <v>5162.36</v>
       </c>
-      <c r="O67" t="s" s="2">
+      <c r="O67" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P67" s="7">
@@ -5342,7 +5369,7 @@
       <c r="A68" t="s" s="2">
         <v>110</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="4">
         <v>12295972</v>
       </c>
       <c r="C68" t="s" s="2">
@@ -5354,28 +5381,28 @@
       <c r="E68" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
       <c r="I68" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J68" s="3">
+      <c r="J68" s="4">
         <v>1002088146</v>
       </c>
-      <c r="K68" s="4">
+      <c r="K68" s="5">
         <v>40309</v>
       </c>
-      <c r="L68" s="3">
+      <c r="L68" s="4">
         <v>2459</v>
       </c>
-      <c r="M68" s="5">
+      <c r="M68" s="6">
         <v>2528.84</v>
       </c>
-      <c r="N68" s="5">
+      <c r="N68" s="6">
         <v>16585.15</v>
       </c>
-      <c r="O68" t="s" s="2">
+      <c r="O68" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P68" s="7">
@@ -5398,7 +5425,7 @@
       <c r="A69" t="s" s="2">
         <v>110</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="4">
         <v>12295972</v>
       </c>
       <c r="C69" t="s" s="2">
@@ -5410,28 +5437,28 @@
       <c r="E69" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
       <c r="I69" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J69" s="3">
+      <c r="J69" s="4">
         <v>1040166253</v>
       </c>
-      <c r="K69" s="4">
+      <c r="K69" s="5">
         <v>40309</v>
       </c>
-      <c r="L69" s="3">
+      <c r="L69" s="4">
         <v>2428</v>
       </c>
-      <c r="M69" s="5">
+      <c r="M69" s="6">
         <v>21539.99</v>
       </c>
-      <c r="N69" s="5">
+      <c r="N69" s="6">
         <v>141599.24</v>
       </c>
-      <c r="O69" t="s" s="2">
+      <c r="O69" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P69" s="7">
@@ -5454,7 +5481,7 @@
       <c r="A70" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="4">
         <v>18034432</v>
       </c>
       <c r="C70" t="s" s="2">
@@ -5466,28 +5493,28 @@
       <c r="E70" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
       <c r="I70" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J70" s="3">
+      <c r="J70" s="4">
         <v>1040238616</v>
       </c>
-      <c r="K70" s="4">
+      <c r="K70" s="5">
         <v>40485</v>
       </c>
-      <c r="L70" s="3">
+      <c r="L70" s="4">
         <v>2283</v>
       </c>
-      <c r="M70" s="5">
+      <c r="M70" s="6">
         <v>670.92</v>
       </c>
-      <c r="N70" s="5">
+      <c r="N70" s="6">
         <v>4401.53</v>
       </c>
-      <c r="O70" t="s" s="2">
+      <c r="O70" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P70" s="7">
@@ -5510,7 +5537,7 @@
       <c r="A71" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="4">
         <v>5129721</v>
       </c>
       <c r="C71" t="s" s="2">
@@ -5522,28 +5549,28 @@
       <c r="E71" t="s" s="2">
         <v>117</v>
       </c>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
       <c r="I71" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J71" s="3">
+      <c r="J71" s="4">
         <v>202737</v>
       </c>
-      <c r="K71" s="4">
+      <c r="K71" s="5">
         <v>40432</v>
       </c>
-      <c r="L71" s="3">
+      <c r="L71" s="4">
         <v>2336</v>
       </c>
-      <c r="M71" s="5">
+      <c r="M71" s="6">
         <v>7324.65</v>
       </c>
-      <c r="N71" s="5">
+      <c r="N71" s="6">
         <v>12261.54</v>
       </c>
-      <c r="O71" t="s" s="2">
+      <c r="O71" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P71" s="7">
@@ -5566,7 +5593,7 @@
       <c r="A72" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="4">
         <v>5905827</v>
       </c>
       <c r="C72" t="s" s="2">
@@ -5578,28 +5605,28 @@
       <c r="E72" t="s" s="2">
         <v>120</v>
       </c>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
       <c r="I72" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J72" s="3">
+      <c r="J72" s="4">
         <v>1030336796</v>
       </c>
-      <c r="K72" s="4">
+      <c r="K72" s="5">
         <v>40832</v>
       </c>
-      <c r="L72" s="3">
+      <c r="L72" s="4">
         <v>1936</v>
       </c>
-      <c r="M72" s="5">
+      <c r="M72" s="6">
         <v>4780.32</v>
       </c>
-      <c r="N72" s="5">
+      <c r="N72" s="6">
         <v>18797.86</v>
       </c>
-      <c r="O72" t="s" s="2">
+      <c r="O72" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P72" s="7">
@@ -5622,7 +5649,7 @@
       <c r="A73" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="4">
         <v>18131747</v>
       </c>
       <c r="C73" t="s" s="2">
@@ -5634,28 +5661,28 @@
       <c r="E73" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
       <c r="I73" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J73" s="3">
+      <c r="J73" s="4">
         <v>1003087773</v>
       </c>
-      <c r="K73" s="4">
+      <c r="K73" s="5">
         <v>40730</v>
       </c>
-      <c r="L73" s="3">
+      <c r="L73" s="4">
         <v>2033</v>
       </c>
-      <c r="M73" s="5">
+      <c r="M73" s="6">
         <v>51235.05</v>
       </c>
-      <c r="N73" s="5">
+      <c r="N73" s="6">
         <v>278353.98</v>
       </c>
-      <c r="O73" t="s" s="2">
+      <c r="O73" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P73" s="7">
@@ -5678,7 +5705,7 @@
       <c r="A74" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="4">
         <v>18131747</v>
       </c>
       <c r="C74" t="s" s="2">
@@ -5690,28 +5717,28 @@
       <c r="E74" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
       <c r="I74" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J74" s="3">
+      <c r="J74" s="4">
         <v>1003425573</v>
       </c>
-      <c r="K74" s="4">
+      <c r="K74" s="5">
         <v>40730</v>
       </c>
-      <c r="L74" s="3">
+      <c r="L74" s="4">
         <v>2038</v>
       </c>
-      <c r="M74" s="5">
+      <c r="M74" s="6">
         <v>637.03</v>
       </c>
-      <c r="N74" s="5">
+      <c r="N74" s="6">
         <v>3450.4</v>
       </c>
-      <c r="O74" t="s" s="2">
+      <c r="O74" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P74" s="7">
@@ -5734,7 +5761,7 @@
       <c r="A75" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="4">
         <v>18131747</v>
       </c>
       <c r="C75" t="s" s="2">
@@ -5746,28 +5773,28 @@
       <c r="E75" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
       <c r="I75" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J75" s="3">
+      <c r="J75" s="4">
         <v>1003462014</v>
       </c>
-      <c r="K75" s="4">
+      <c r="K75" s="5">
         <v>40730</v>
       </c>
-      <c r="L75" s="3">
+      <c r="L75" s="4">
         <v>2010</v>
       </c>
-      <c r="M75" s="5">
+      <c r="M75" s="6">
         <v>496.38</v>
       </c>
-      <c r="N75" s="5">
+      <c r="N75" s="6">
         <v>2689.93</v>
       </c>
-      <c r="O75" t="s" s="2">
+      <c r="O75" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P75" s="7">
@@ -5790,7 +5817,7 @@
       <c r="A76" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="4">
         <v>21792045</v>
       </c>
       <c r="C76" t="s" s="2">
@@ -5802,28 +5829,28 @@
       <c r="E76" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
       <c r="I76" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J76" s="3">
+      <c r="J76" s="4">
         <v>1001802545</v>
       </c>
-      <c r="K76" s="4">
+      <c r="K76" s="5">
         <v>40422</v>
       </c>
-      <c r="L76" s="3">
+      <c r="L76" s="4">
         <v>2336</v>
       </c>
-      <c r="M76" s="5">
+      <c r="M76" s="6">
         <v>2061.61</v>
       </c>
-      <c r="N76" s="5">
+      <c r="N76" s="6">
         <v>9901.709999999999</v>
       </c>
-      <c r="O76" t="s" s="2">
+      <c r="O76" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P76" s="7">
@@ -5846,7 +5873,7 @@
       <c r="A77" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="4">
         <v>21792045</v>
       </c>
       <c r="C77" t="s" s="2">
@@ -5858,28 +5885,28 @@
       <c r="E77" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
       <c r="I77" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J77" s="3">
+      <c r="J77" s="4">
         <v>1002050979</v>
       </c>
-      <c r="K77" s="4">
+      <c r="K77" s="5">
         <v>40422</v>
       </c>
-      <c r="L77" s="3">
+      <c r="L77" s="4">
         <v>2336</v>
       </c>
-      <c r="M77" s="5">
+      <c r="M77" s="6">
         <v>13978.75</v>
       </c>
-      <c r="N77" s="5">
+      <c r="N77" s="6">
         <v>66919.34</v>
       </c>
-      <c r="O77" t="s" s="2">
+      <c r="O77" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P77" s="7">
@@ -5902,7 +5929,7 @@
       <c r="A78" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="4">
         <v>21792045</v>
       </c>
       <c r="C78" t="s" s="2">
@@ -5914,28 +5941,28 @@
       <c r="E78" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
       <c r="I78" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J78" s="3">
+      <c r="J78" s="4">
         <v>1002262338</v>
       </c>
-      <c r="K78" s="4">
+      <c r="K78" s="5">
         <v>40422</v>
       </c>
-      <c r="L78" s="3">
+      <c r="L78" s="4">
         <v>2336</v>
       </c>
-      <c r="M78" s="5">
+      <c r="M78" s="6">
         <v>5634.78</v>
       </c>
-      <c r="N78" s="5">
+      <c r="N78" s="6">
         <v>27187.46</v>
       </c>
-      <c r="O78" t="s" s="2">
+      <c r="O78" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P78" s="7">
@@ -5958,7 +5985,7 @@
       <c r="A79" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="4">
         <v>21792045</v>
       </c>
       <c r="C79" t="s" s="2">
@@ -5970,28 +5997,28 @@
       <c r="E79" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
       <c r="I79" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="J79" s="3">
+      <c r="J79" s="4">
         <v>1370091658</v>
       </c>
-      <c r="K79" s="4">
+      <c r="K79" s="5">
         <v>40422</v>
       </c>
-      <c r="L79" s="3">
+      <c r="L79" s="4">
         <v>2346</v>
       </c>
-      <c r="M79" s="5">
+      <c r="M79" s="6">
         <v>1838.79</v>
       </c>
-      <c r="N79" s="5">
+      <c r="N79" s="6">
         <v>8979.719999999999</v>
       </c>
-      <c r="O79" t="s" s="2">
+      <c r="O79" t="s" s="3">
         <v>101</v>
       </c>
       <c r="P79" s="7">

</xml_diff>